<commit_message>
fix show cost price and cost amount in report stock move
</commit_message>
<xml_diff>
--- a/netforce_stock/netforce_stock/reports/report_stock_move.xlsx
+++ b/netforce_stock/netforce_stock/reports/report_stock_move.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>{{title}}</t>
   </si>
@@ -49,6 +49,12 @@
     <t>UoM</t>
   </si>
   <si>
+    <t>Cost Price</t>
+  </si>
+  <si>
+    <t>Cost Amount</t>
+  </si>
+  <si>
     <t>To Location</t>
   </si>
   <si>
@@ -98,6 +104,12 @@
   </si>
   <si>
     <t>{{uom}}</t>
+  </si>
+  <si>
+    <t>{{cost_price}}</t>
+  </si>
+  <si>
+    <t>{{cost_amount}}</t>
   </si>
   <si>
     <t>{{location_to}}</t>
@@ -276,8 +288,8 @@
   </sheetPr>
   <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -291,12 +303,14 @@
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.1989795918367"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.9591836734694"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.02551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="1" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="1" width="15.5612244897959"/>
-    <col collapsed="false" hidden="false" max="973" min="18" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.219387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.2551020408163"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="18.1989795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="1" width="18.1989795918367"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="1" width="15.5612244897959"/>
+    <col collapsed="false" hidden="false" max="975" min="20" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="976" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -304,8 +318,6 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="AKL1" s="0"/>
-      <c r="AKM1" s="0"/>
       <c r="AKN1" s="0"/>
       <c r="AKO1" s="0"/>
       <c r="AKP1" s="0"/>
@@ -359,8 +371,6 @@
     <row r="2" s="3" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="2"/>
-      <c r="AKL2" s="0"/>
-      <c r="AKM2" s="0"/>
       <c r="AKN2" s="0"/>
       <c r="AKO2" s="0"/>
       <c r="AKP2" s="0"/>
@@ -461,8 +471,12 @@
       <c r="Q3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AKL3" s="4"/>
-      <c r="AKM3" s="4"/>
+      <c r="R3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="AKN3" s="4"/>
       <c r="AKO3" s="4"/>
       <c r="AKP3" s="4"/>
@@ -515,7 +529,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -532,60 +546,68 @@
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="9" t="s">
         <v>28</v>
       </c>
+      <c r="K5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="M5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="8" t="s">
         <v>33</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -602,6 +624,8 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>